<commit_message>
them chuc năng thong bao và xem thong bao
</commit_message>
<xml_diff>
--- a/score/GPS/report.xlsx
+++ b/score/GPS/report.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="10">
   <si>
     <t>STT</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>Nội dung</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>yyy</t>
   </si>
 </sst>
 </file>
@@ -85,9 +91,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,13 +422,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -437,6 +447,48 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45272</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45272</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45272</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -444,13 +496,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -466,6 +521,62 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45272</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45273</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45274</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45275</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -473,13 +584,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -495,6 +609,62 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45270</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45273</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45276</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45279</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -502,13 +672,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -524,6 +697,62 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45270</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45271</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45272</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45273</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>